<commit_message>
chapter 3 updated to the end of our video encoder
</commit_message>
<xml_diff>
--- a/project_latex/footnotes.xlsx
+++ b/project_latex/footnotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\master courses and files\master courses\master project\thesis report\parisa master thesis\project_latex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25858B-AF13-462F-85CF-4EA4EC8D6A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596ECAB2-E74D-4652-B26F-08678608B184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{83D7A62A-F015-4500-931D-93DF1FFC8BA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>task specific</t>
   </si>
@@ -196,6 +196,24 @@
   </si>
   <si>
     <t>Overfitting</t>
+  </si>
+  <si>
+    <t>hyper parameter</t>
+  </si>
+  <si>
+    <t>Stochastic Weight Averaging</t>
+  </si>
+  <si>
+    <t>Prompt selection</t>
+  </si>
+  <si>
+    <t>classifier</t>
+  </si>
+  <si>
+    <t>Frozen</t>
+  </si>
+  <si>
+    <t>Class feature (CLS)</t>
   </si>
 </sst>
 </file>
@@ -548,10 +566,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CD2731-45ED-45A9-A4E5-00F077C0CA39}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -844,6 +862,36 @@
         <v>56</v>
       </c>
     </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
end of chapter 3
</commit_message>
<xml_diff>
--- a/project_latex/footnotes.xlsx
+++ b/project_latex/footnotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\master courses and files\master courses\master project\thesis report\parisa master thesis\project_latex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596ECAB2-E74D-4652-B26F-08678608B184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D340A8-9E2A-495E-A14C-1F25D384233B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{83D7A62A-F015-4500-931D-93DF1FFC8BA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>task specific</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Class feature (CLS)</t>
+  </si>
+  <si>
+    <t>embedding size</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CD2731-45ED-45A9-A4E5-00F077C0CA39}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -892,6 +895,11 @@
         <v>62</v>
       </c>
     </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edditing some parts that behnam said
</commit_message>
<xml_diff>
--- a/project_latex/footnotes.xlsx
+++ b/project_latex/footnotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\master courses and files\master courses\master project\thesis report\parisa master thesis\project_latex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D340A8-9E2A-495E-A14C-1F25D384233B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E8EC0B-DD4B-4D37-8EEA-BA6D7D8708D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{83D7A62A-F015-4500-931D-93DF1FFC8BA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>task specific</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>embedding size</t>
+  </si>
+  <si>
+    <t>Task identity</t>
+  </si>
+  <si>
+    <t>Technique</t>
   </si>
 </sst>
 </file>
@@ -569,10 +575,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CD2731-45ED-45A9-A4E5-00F077C0CA39}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -900,6 +906,16 @@
         <v>63</v>
       </c>
     </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>